<commit_message>
cambio moneda en reportes caja y flujo estimacion costo
</commit_message>
<xml_diff>
--- a/backend/src/tmp/ExcelCaja.xlsx
+++ b/backend/src/tmp/ExcelCaja.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Mes 1</t>
   </si>
@@ -22,6 +22,9 @@
     <t>Mes 3</t>
   </si>
   <si>
+    <t>Mes 4</t>
+  </si>
+  <si>
     <t>Ingresos(*)</t>
   </si>
   <si>
@@ -43,16 +46,7 @@
     <t>Egresos(*)</t>
   </si>
   <si>
-    <t>Egreso 1</t>
-  </si>
-  <si>
-    <t>Egreso 2</t>
-  </si>
-  <si>
-    <t>Egreso 3</t>
-  </si>
-  <si>
-    <t>Egreso 4</t>
+    <t>Ingenieros</t>
   </si>
   <si>
     <t>Total Egresos</t>
@@ -456,14 +450,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E12"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="4" width="10" customWidth="1"/>
+    <col min="2" max="5" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -473,102 +467,123 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>12500</v>
       </c>
       <c r="C3">
-        <v>69133</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>4488000</v>
       </c>
       <c r="C4">
-        <v>100056</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>80801</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
-        <v>59980</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
+        <v>4500500</v>
       </c>
       <c r="C7" s="1">
-        <v>309970</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>8976</v>
       </c>
       <c r="C9">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -576,79 +591,46 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>20000</v>
+        <v>13464</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>30000</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>8976</v>
+      </c>
+      <c r="C11" s="1">
+        <v>13464</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>40000</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>60000</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1">
-        <v>160000</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="1">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1">
-        <v>149970</v>
-      </c>
-      <c r="D15" s="1">
+      <c r="B12" s="1">
+        <v>4491524</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-13464</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
pipipi por que chung???
</commit_message>
<xml_diff>
--- a/backend/src/tmp/ExcelCaja.xlsx
+++ b/backend/src/tmp/ExcelCaja.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Mes 1</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>Egresos(*)</t>
-  </si>
-  <si>
-    <t>Ingenieros</t>
   </si>
   <si>
     <t>Total Egresos</t>
@@ -450,7 +447,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E10"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
@@ -570,67 +567,33 @@
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
-        <v>8976</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>13464</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1">
-        <v>8976</v>
-      </c>
-      <c r="C11" s="1">
-        <v>13464</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1">
-        <v>4491524</v>
-      </c>
-      <c r="C12" s="1">
-        <v>-13464</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1">
+      <c r="B10" s="1">
+        <v>4500500</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>